<commit_message>
corrected rna sample numbers in s1CDNASample_hbrown_08.15.19
</commit_message>
<xml_diff>
--- a/s1cDNASample/s1CDNASample_hbrown_08.15.19.xlsx
+++ b/s1cDNASample/s1CDNASample_hbrown_08.15.19.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hollybrown/database_files/s1cDNASample/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DAF2FF-0F9C-814B-9597-E860F78D270A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E1CDF7E-D22F-A249-8D72-233F54A68FC1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="16380" windowHeight="16760" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -459,7 +459,7 @@
   <dimension ref="A1:Z27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I27"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -525,7 +525,7 @@
         <v>11</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -573,7 +573,7 @@
         <v>11</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -605,7 +605,7 @@
         <v>11</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>29</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -637,7 +637,7 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>30</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -669,7 +669,7 @@
         <v>11</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>31</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -701,7 +701,7 @@
         <v>11</v>
       </c>
       <c r="C7">
-        <v>6</v>
+        <v>32</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -733,7 +733,7 @@
         <v>11</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -765,7 +765,7 @@
         <v>11</v>
       </c>
       <c r="C9">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -797,7 +797,7 @@
         <v>11</v>
       </c>
       <c r="C10">
-        <v>9</v>
+        <v>35</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -829,7 +829,7 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -861,7 +861,7 @@
         <v>11</v>
       </c>
       <c r="C12">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -893,7 +893,7 @@
         <v>11</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>38</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -925,7 +925,7 @@
         <v>11</v>
       </c>
       <c r="C14">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -957,7 +957,7 @@
         <v>11</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -989,7 +989,7 @@
         <v>11</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -1021,7 +1021,7 @@
         <v>11</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -1053,7 +1053,7 @@
         <v>11</v>
       </c>
       <c r="C18">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -1085,7 +1085,7 @@
         <v>11</v>
       </c>
       <c r="C19">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>12</v>
@@ -1117,7 +1117,7 @@
         <v>11</v>
       </c>
       <c r="C20">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>12</v>
@@ -1149,7 +1149,7 @@
         <v>11</v>
       </c>
       <c r="C21">
-        <v>20</v>
+        <v>46</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>12</v>
@@ -1181,7 +1181,7 @@
         <v>11</v>
       </c>
       <c r="C22">
-        <v>21</v>
+        <v>47</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>12</v>
@@ -1213,7 +1213,7 @@
         <v>11</v>
       </c>
       <c r="C23">
-        <v>22</v>
+        <v>48</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>12</v>
@@ -1245,7 +1245,7 @@
         <v>11</v>
       </c>
       <c r="C24">
-        <v>23</v>
+        <v>49</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>12</v>
@@ -1277,7 +1277,7 @@
         <v>11</v>
       </c>
       <c r="C25">
-        <v>24</v>
+        <v>50</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>12</v>
@@ -1309,7 +1309,7 @@
         <v>11</v>
       </c>
       <c r="C26">
-        <v>25</v>
+        <v>51</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>12</v>
@@ -1341,7 +1341,7 @@
         <v>11</v>
       </c>
       <c r="C27">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>12</v>

</xml_diff>